<commit_message>
started work on lab2. Trying to figure out handles
</commit_message>
<xml_diff>
--- a/lab1/charts.xlsx
+++ b/lab1/charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="2140" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bandwidth" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>PROCESSORS</t>
+  </si>
+  <si>
+    <t>FLOPS</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63,8 +74,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -73,11 +86,13 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -848,6 +863,218 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Floating Point Operations per Second vs.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Processors employed</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>flops!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>flops!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.71625940752602E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.54235532678209E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.39763545484838E9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.09401098352471E9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8215970400269E9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.49671029595664E9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.15895290034705E9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8657819025522E9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2145779304"/>
+        <c:axId val="-2120673304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2145779304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Processors</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2120673304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2120673304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>FLOPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2145779304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -866,6 +1093,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1" title="Bandwidth Profile of AWS Server"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1207,7 +1469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -2019,13 +2281,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>671625940.75260198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>654235532.67820895</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1397635454.8483801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2094010983.5247099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2821597040.0268998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3496710295.9566398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>4158952900.3470502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>4865781902.5522003</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>